<commit_message>
PAYS OK ! NB LIGNES OK !
</commit_message>
<xml_diff>
--- a/Base de données/insert into/PAYS.xlsx
+++ b/Base de données/insert into/PAYS.xlsx
@@ -16,147 +16,144 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="47">
-  <si>
-    <t>PAYS</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>GERMANY</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>FRANCE</t>
-  </si>
-  <si>
-    <t>NEW-ZEALAND</t>
-  </si>
-  <si>
-    <t>SWITZERLAND</t>
-  </si>
-  <si>
-    <t>CANADA</t>
-  </si>
-  <si>
-    <t>DENMARK</t>
-  </si>
-  <si>
-    <t>AUSTRALIA</t>
-  </si>
-  <si>
-    <t>ITALY</t>
-  </si>
-  <si>
-    <t>SPAIN</t>
-  </si>
-  <si>
-    <t>NETHERLANDS</t>
-  </si>
-  <si>
-    <t>TURKEY</t>
-  </si>
-  <si>
-    <t>AUSTRIA</t>
-  </si>
-  <si>
-    <t>POLAND</t>
-  </si>
-  <si>
-    <t>JAPAN</t>
-  </si>
-  <si>
-    <t>CROATIA</t>
-  </si>
-  <si>
-    <t>RUSSIA</t>
-  </si>
-  <si>
-    <t>SWEDEN</t>
-  </si>
-  <si>
-    <t>NORWAY</t>
-  </si>
-  <si>
-    <t>INDIA</t>
-  </si>
-  <si>
-    <t>BELGIUM</t>
-  </si>
-  <si>
-    <t>IRELAND</t>
-  </si>
-  <si>
-    <t>ISRAEL</t>
-  </si>
-  <si>
-    <t>HUNGARY</t>
-  </si>
-  <si>
-    <t>SINGAPORE</t>
-  </si>
-  <si>
-    <t>IRAN</t>
-  </si>
-  <si>
-    <t>GREECE</t>
-  </si>
-  <si>
-    <t>CZECHOSLOVAKIA</t>
-  </si>
-  <si>
-    <t>COLOMBIA</t>
-  </si>
-  <si>
-    <t>CHINA</t>
-  </si>
-  <si>
-    <t>YUGOSLAVIA</t>
-  </si>
-  <si>
-    <t>UKRAINE</t>
-  </si>
-  <si>
-    <t>SOUTH-AFRICA</t>
-  </si>
-  <si>
-    <t>SLOVAKIA</t>
-  </si>
-  <si>
-    <t>ROMANIA</t>
-  </si>
-  <si>
-    <t>PORTUGAL</t>
-  </si>
-  <si>
-    <t>NIGERIA</t>
-  </si>
-  <si>
-    <t>HONG-KONG</t>
-  </si>
-  <si>
-    <t>GEORGIA</t>
-  </si>
-  <si>
-    <t>FINLAND</t>
-  </si>
-  <si>
-    <t>ESTONIA</t>
-  </si>
-  <si>
-    <t>EGYPT</t>
-  </si>
-  <si>
-    <t>BOSNIA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="46">
   <si>
     <t>INSERT INTO PAYS VALUES ('</t>
   </si>
   <si>
     <t>');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GERMANY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRANCE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW-ZEALAND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWITZERLAND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CANADA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DENMARK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUSTRALIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITALY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPAIN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NETHERLANDS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TURKEY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUSTRIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLAND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JAPAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CROATIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUSSIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWEDEN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NORWAY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BELGIUM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRELAND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISRAEL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUNGARY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SINGAPORE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GREECE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZECHOSLOVAKIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLOMBIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHINA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">YUGOSLAVIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UKRAINE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOUTH-AFRICA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLOVAKIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROMANIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PORTUGAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIGERIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HONG-KONG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEORGIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FINLAND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTONIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGYPT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOSNIA </t>
   </si>
 </sst>
 </file>
@@ -497,504 +494,500 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A2:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
         <v>45</v>
       </c>
-      <c r="B45" t="s">
-        <v>44</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>